<commit_message>
Docs: added missing variables from Outputs
</commit_message>
<xml_diff>
--- a/utilities/RTP/Emissions/Off Model Calculators/models/Variable_locations.xlsx
+++ b/utilities/RTP/Emissions/Off Model Calculators/models/Variable_locations.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\63330\Documents\projects\MTC\travel-model-one\utilities\RTP\Emissions\Off Model Calculators\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F0F37C-4B12-48B6-A7BF-BDB2C021B42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C24ACD-190A-4EAF-BCFD-D6515912F2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35232" yWindow="0" windowWidth="12480" windowHeight="13200" xr2:uid="{BC60942D-DD94-4578-9A2D-7D64A567FAF1}"/>
+    <workbookView xWindow="22944" yWindow="0" windowWidth="12480" windowHeight="13200" xr2:uid="{BC60942D-DD94-4578-9A2D-7D64A567FAF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$225</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$231</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="481">
   <si>
     <t>VMT_displaced_conventional</t>
   </si>
@@ -1443,13 +1443,52 @@
   </si>
   <si>
     <t>D13</t>
+  </si>
+  <si>
+    <t>ACCII_toggle</t>
+  </si>
+  <si>
+    <t>B21</t>
+  </si>
+  <si>
+    <t>B24</t>
+  </si>
+  <si>
+    <t>Number_L2_incentivized</t>
+  </si>
+  <si>
+    <t>Number_DCFC_50kW_incentivized</t>
+  </si>
+  <si>
+    <t>Number_DCFC_150kW_incentivized</t>
+  </si>
+  <si>
+    <t>Number_DCFC_250kW_incentivized</t>
+  </si>
+  <si>
+    <t>Number_DCFC_350kW_incentivized</t>
+  </si>
+  <si>
+    <t>B26</t>
+  </si>
+  <si>
+    <t>B27</t>
+  </si>
+  <si>
+    <t>B28</t>
+  </si>
+  <si>
+    <t>B29</t>
+  </si>
+  <si>
+    <t>B30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1467,6 +1506,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1492,9 +1537,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1829,10 +1875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC65239-A95B-4A8F-9499-495761FDA170}">
-  <dimension ref="A1:E225"/>
+  <dimension ref="A1:E231"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -3569,13 +3615,10 @@
         <v>28</v>
       </c>
       <c r="C103" t="s">
-        <v>286</v>
-      </c>
-      <c r="D103" t="s">
-        <v>271</v>
+        <v>468</v>
       </c>
       <c r="E103" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3586,10 +3629,10 @@
         <v>28</v>
       </c>
       <c r="C104" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D104" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E104" t="s">
         <v>49</v>
@@ -3603,10 +3646,10 @@
         <v>28</v>
       </c>
       <c r="C105" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D105" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E105" t="s">
         <v>252</v>
@@ -3620,10 +3663,10 @@
         <v>28</v>
       </c>
       <c r="C106" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D106" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E106" t="s">
         <v>276</v>
@@ -3637,10 +3680,10 @@
         <v>28</v>
       </c>
       <c r="C107" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D107" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E107" t="s">
         <v>277</v>
@@ -3654,13 +3697,13 @@
         <v>28</v>
       </c>
       <c r="C108" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D108" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E108" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3671,10 +3714,10 @@
         <v>28</v>
       </c>
       <c r="C109" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D109" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E109" t="s">
         <v>298</v>
@@ -3688,10 +3731,10 @@
         <v>28</v>
       </c>
       <c r="C110" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D110" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E110" t="s">
         <v>299</v>
@@ -3705,10 +3748,10 @@
         <v>28</v>
       </c>
       <c r="C111" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D111" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E111" t="s">
         <v>300</v>
@@ -3722,10 +3765,10 @@
         <v>28</v>
       </c>
       <c r="C112" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D112" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E112" t="s">
         <v>301</v>
@@ -3739,13 +3782,13 @@
         <v>28</v>
       </c>
       <c r="C113" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="D113" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E113" t="s">
-        <v>302</v>
+        <v>469</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3756,10 +3799,10 @@
         <v>28</v>
       </c>
       <c r="C114" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="D114" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E114" t="s">
         <v>303</v>
@@ -3773,13 +3816,13 @@
         <v>28</v>
       </c>
       <c r="C115" t="s">
-        <v>18</v>
+        <v>297</v>
       </c>
       <c r="D115" t="s">
-        <v>192</v>
+        <v>284</v>
       </c>
       <c r="E115" t="s">
-        <v>139</v>
+        <v>470</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -3790,13 +3833,13 @@
         <v>28</v>
       </c>
       <c r="C116" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D116" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="E116" t="s">
-        <v>140</v>
+        <v>304</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -3807,13 +3850,13 @@
         <v>28</v>
       </c>
       <c r="C117" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D117" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="E117" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -3824,13 +3867,13 @@
         <v>28</v>
       </c>
       <c r="C118" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D118" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="E118" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -3841,13 +3884,13 @@
         <v>28</v>
       </c>
       <c r="C119" t="s">
-        <v>235</v>
+        <v>21</v>
       </c>
       <c r="D119" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E119" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -3858,109 +3901,100 @@
         <v>28</v>
       </c>
       <c r="C120" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D120" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E120" t="s">
-        <v>307</v>
+        <v>432</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>463</v>
+        <v>269</v>
       </c>
       <c r="B121" t="s">
         <v>28</v>
       </c>
       <c r="C121" t="s">
-        <v>12</v>
+        <v>236</v>
+      </c>
+      <c r="D121" t="s">
+        <v>212</v>
       </c>
       <c r="E121" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>463</v>
+        <v>269</v>
       </c>
       <c r="B122" t="s">
         <v>28</v>
       </c>
-      <c r="C122" t="s">
-        <v>13</v>
+      <c r="C122" s="2" t="s">
+        <v>471</v>
       </c>
       <c r="E122" t="s">
-        <v>449</v>
+        <v>476</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>463</v>
+        <v>269</v>
       </c>
       <c r="B123" t="s">
         <v>28</v>
       </c>
-      <c r="C123" t="s">
-        <v>387</v>
-      </c>
-      <c r="D123" t="s">
-        <v>310</v>
+      <c r="C123" s="2" t="s">
+        <v>472</v>
       </c>
       <c r="E123" t="s">
-        <v>40</v>
+        <v>477</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>463</v>
+        <v>269</v>
       </c>
       <c r="B124" t="s">
         <v>28</v>
       </c>
-      <c r="C124" t="s">
-        <v>388</v>
-      </c>
-      <c r="D124" t="s">
-        <v>311</v>
+      <c r="C124" s="2" t="s">
+        <v>473</v>
       </c>
       <c r="E124" t="s">
-        <v>41</v>
+        <v>478</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>463</v>
+        <v>269</v>
       </c>
       <c r="B125" t="s">
         <v>28</v>
       </c>
-      <c r="C125" t="s">
-        <v>389</v>
-      </c>
-      <c r="D125" t="s">
-        <v>312</v>
+      <c r="C125" s="2" t="s">
+        <v>474</v>
       </c>
       <c r="E125" t="s">
-        <v>251</v>
+        <v>479</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>463</v>
+        <v>269</v>
       </c>
       <c r="B126" t="s">
         <v>28</v>
       </c>
-      <c r="C126" t="s">
-        <v>390</v>
-      </c>
-      <c r="D126" t="s">
-        <v>313</v>
+      <c r="C126" s="2" t="s">
+        <v>475</v>
       </c>
       <c r="E126" t="s">
-        <v>43</v>
+        <v>480</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -3971,13 +4005,10 @@
         <v>28</v>
       </c>
       <c r="C127" t="s">
-        <v>391</v>
-      </c>
-      <c r="D127" t="s">
-        <v>314</v>
+        <v>12</v>
       </c>
       <c r="E127" t="s">
-        <v>46</v>
+        <v>448</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -3988,13 +4019,10 @@
         <v>28</v>
       </c>
       <c r="C128" t="s">
-        <v>394</v>
-      </c>
-      <c r="D128" t="s">
-        <v>315</v>
+        <v>13</v>
       </c>
       <c r="E128" t="s">
-        <v>49</v>
+        <v>449</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4005,13 +4033,13 @@
         <v>28</v>
       </c>
       <c r="C129" t="s">
-        <v>429</v>
+        <v>387</v>
       </c>
       <c r="D129" t="s">
-        <v>428</v>
+        <v>310</v>
       </c>
       <c r="E129" t="s">
-        <v>252</v>
+        <v>40</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -4022,13 +4050,13 @@
         <v>28</v>
       </c>
       <c r="C130" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="D130" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="E130" t="s">
-        <v>276</v>
+        <v>41</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -4039,13 +4067,13 @@
         <v>28</v>
       </c>
       <c r="C131" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D131" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="E131" t="s">
-        <v>277</v>
+        <v>251</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -4056,13 +4084,13 @@
         <v>28</v>
       </c>
       <c r="C132" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="D132" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="E132" t="s">
-        <v>253</v>
+        <v>43</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -4073,13 +4101,13 @@
         <v>28</v>
       </c>
       <c r="C133" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="D133" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E133" t="s">
-        <v>254</v>
+        <v>46</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -4090,13 +4118,13 @@
         <v>28</v>
       </c>
       <c r="C134" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D134" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="E134" t="s">
-        <v>298</v>
+        <v>49</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -4107,13 +4135,13 @@
         <v>28</v>
       </c>
       <c r="C135" t="s">
-        <v>398</v>
+        <v>429</v>
       </c>
       <c r="D135" t="s">
-        <v>321</v>
+        <v>428</v>
       </c>
       <c r="E135" t="s">
-        <v>300</v>
+        <v>252</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -4124,13 +4152,13 @@
         <v>28</v>
       </c>
       <c r="C136" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="D136" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="E136" t="s">
-        <v>301</v>
+        <v>276</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -4141,13 +4169,13 @@
         <v>28</v>
       </c>
       <c r="C137" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="D137" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="E137" t="s">
-        <v>302</v>
+        <v>277</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -4158,13 +4186,13 @@
         <v>28</v>
       </c>
       <c r="C138" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="D138" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="E138" t="s">
-        <v>303</v>
+        <v>253</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -4175,13 +4203,13 @@
         <v>28</v>
       </c>
       <c r="C139" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="D139" t="s">
-        <v>349</v>
+        <v>319</v>
       </c>
       <c r="E139" t="s">
-        <v>135</v>
+        <v>254</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4192,13 +4220,13 @@
         <v>28</v>
       </c>
       <c r="C140" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="D140" t="s">
-        <v>370</v>
+        <v>320</v>
       </c>
       <c r="E140" t="s">
-        <v>136</v>
+        <v>298</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -4209,13 +4237,13 @@
         <v>28</v>
       </c>
       <c r="C141" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="D141" t="s">
-        <v>350</v>
+        <v>321</v>
       </c>
       <c r="E141" t="s">
-        <v>259</v>
+        <v>300</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -4226,13 +4254,13 @@
         <v>28</v>
       </c>
       <c r="C142" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="D142" t="s">
-        <v>371</v>
+        <v>322</v>
       </c>
       <c r="E142" t="s">
-        <v>430</v>
+        <v>301</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -4243,13 +4271,13 @@
         <v>28</v>
       </c>
       <c r="C143" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="D143" t="s">
-        <v>351</v>
+        <v>323</v>
       </c>
       <c r="E143" t="s">
-        <v>137</v>
+        <v>302</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4260,13 +4288,13 @@
         <v>28</v>
       </c>
       <c r="C144" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="D144" t="s">
-        <v>372</v>
+        <v>324</v>
       </c>
       <c r="E144" t="s">
-        <v>138</v>
+        <v>303</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -4277,13 +4305,13 @@
         <v>28</v>
       </c>
       <c r="C145" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
       <c r="D145" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="E145" t="s">
-        <v>260</v>
+        <v>135</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -4294,13 +4322,13 @@
         <v>28</v>
       </c>
       <c r="C146" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="D146" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E146" t="s">
-        <v>431</v>
+        <v>136</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -4311,13 +4339,13 @@
         <v>28</v>
       </c>
       <c r="C147" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="D147" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E147" t="s">
-        <v>304</v>
+        <v>259</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -4328,13 +4356,13 @@
         <v>28</v>
       </c>
       <c r="C148" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="D148" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E148" t="s">
-        <v>305</v>
+        <v>430</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -4345,13 +4373,13 @@
         <v>28</v>
       </c>
       <c r="C149" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="D149" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="E149" t="s">
-        <v>306</v>
+        <v>137</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -4362,13 +4390,13 @@
         <v>28</v>
       </c>
       <c r="C150" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
       <c r="D150" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E150" t="s">
-        <v>307</v>
+        <v>138</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -4379,13 +4407,13 @@
         <v>28</v>
       </c>
       <c r="C151" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="D151" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="E151" t="s">
-        <v>432</v>
+        <v>260</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -4396,13 +4424,13 @@
         <v>28</v>
       </c>
       <c r="C152" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="D152" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E152" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4413,13 +4441,13 @@
         <v>28</v>
       </c>
       <c r="C153" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D153" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="E153" t="s">
-        <v>434</v>
+        <v>304</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4430,13 +4458,13 @@
         <v>28</v>
       </c>
       <c r="C154" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="D154" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E154" t="s">
-        <v>435</v>
+        <v>305</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -4447,13 +4475,13 @@
         <v>28</v>
       </c>
       <c r="C155" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D155" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="E155" t="s">
-        <v>436</v>
+        <v>306</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -4464,13 +4492,13 @@
         <v>28</v>
       </c>
       <c r="C156" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="D156" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E156" t="s">
-        <v>437</v>
+        <v>307</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4481,13 +4509,13 @@
         <v>28</v>
       </c>
       <c r="C157" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D157" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E157" t="s">
-        <v>141</v>
+        <v>432</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -4498,13 +4526,13 @@
         <v>28</v>
       </c>
       <c r="C158" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="D158" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E158" t="s">
-        <v>142</v>
+        <v>433</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4515,13 +4543,13 @@
         <v>28</v>
       </c>
       <c r="C159" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
       <c r="D159" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="E159" t="s">
-        <v>143</v>
+        <v>434</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -4532,13 +4560,13 @@
         <v>28</v>
       </c>
       <c r="C160" t="s">
-        <v>410</v>
+        <v>425</v>
       </c>
       <c r="D160" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E160" t="s">
-        <v>144</v>
+        <v>435</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4549,13 +4577,13 @@
         <v>28</v>
       </c>
       <c r="C161" t="s">
-        <v>408</v>
+        <v>421</v>
       </c>
       <c r="D161" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="E161" t="s">
-        <v>145</v>
+        <v>436</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -4566,13 +4594,13 @@
         <v>28</v>
       </c>
       <c r="C162" t="s">
-        <v>409</v>
+        <v>422</v>
       </c>
       <c r="D162" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="E162" t="s">
-        <v>146</v>
+        <v>437</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -4583,13 +4611,13 @@
         <v>28</v>
       </c>
       <c r="C163" t="s">
-        <v>407</v>
+        <v>423</v>
       </c>
       <c r="D163" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E163" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -4600,13 +4628,13 @@
         <v>28</v>
       </c>
       <c r="C164" t="s">
-        <v>406</v>
+        <v>424</v>
       </c>
       <c r="D164" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="E164" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -4617,13 +4645,13 @@
         <v>28</v>
       </c>
       <c r="C165" t="s">
-        <v>16</v>
+        <v>411</v>
       </c>
       <c r="D165" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="E165" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -4634,13 +4662,13 @@
         <v>28</v>
       </c>
       <c r="C166" t="s">
-        <v>17</v>
+        <v>410</v>
       </c>
       <c r="D166" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="E166" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -4651,13 +4679,13 @@
         <v>28</v>
       </c>
       <c r="C167" t="s">
-        <v>18</v>
+        <v>408</v>
       </c>
       <c r="D167" t="s">
-        <v>192</v>
+        <v>360</v>
       </c>
       <c r="E167" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -4668,13 +4696,13 @@
         <v>28</v>
       </c>
       <c r="C168" t="s">
-        <v>19</v>
+        <v>409</v>
       </c>
       <c r="D168" t="s">
-        <v>209</v>
+        <v>381</v>
       </c>
       <c r="E168" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -4685,13 +4713,13 @@
         <v>28</v>
       </c>
       <c r="C169" t="s">
-        <v>20</v>
+        <v>407</v>
       </c>
       <c r="D169" t="s">
-        <v>193</v>
+        <v>361</v>
       </c>
       <c r="E169" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -4702,13 +4730,13 @@
         <v>28</v>
       </c>
       <c r="C170" t="s">
-        <v>21</v>
+        <v>406</v>
       </c>
       <c r="D170" t="s">
-        <v>210</v>
+        <v>382</v>
       </c>
       <c r="E170" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -4719,13 +4747,13 @@
         <v>28</v>
       </c>
       <c r="C171" t="s">
-        <v>366</v>
+        <v>16</v>
       </c>
       <c r="D171" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E171" t="s">
-        <v>438</v>
+        <v>149</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -4736,13 +4764,13 @@
         <v>28</v>
       </c>
       <c r="C172" t="s">
-        <v>367</v>
+        <v>17</v>
       </c>
       <c r="D172" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E172" t="s">
-        <v>439</v>
+        <v>150</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -4753,13 +4781,13 @@
         <v>28</v>
       </c>
       <c r="C173" t="s">
-        <v>368</v>
+        <v>18</v>
       </c>
       <c r="D173" t="s">
-        <v>364</v>
+        <v>192</v>
       </c>
       <c r="E173" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -4770,13 +4798,13 @@
         <v>28</v>
       </c>
       <c r="C174" t="s">
-        <v>369</v>
+        <v>19</v>
       </c>
       <c r="D174" t="s">
-        <v>385</v>
+        <v>209</v>
       </c>
       <c r="E174" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -4787,13 +4815,13 @@
         <v>28</v>
       </c>
       <c r="C175" t="s">
-        <v>235</v>
+        <v>20</v>
       </c>
       <c r="D175" t="s">
-        <v>365</v>
+        <v>193</v>
       </c>
       <c r="E175" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -4804,13 +4832,13 @@
         <v>28</v>
       </c>
       <c r="C176" t="s">
-        <v>236</v>
+        <v>21</v>
       </c>
       <c r="D176" t="s">
-        <v>386</v>
+        <v>210</v>
       </c>
       <c r="E176" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -4821,10 +4849,13 @@
         <v>28</v>
       </c>
       <c r="C177" t="s">
-        <v>458</v>
+        <v>366</v>
+      </c>
+      <c r="D177" t="s">
+        <v>363</v>
       </c>
       <c r="E177" t="s">
-        <v>133</v>
+        <v>438</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -4835,112 +4866,109 @@
         <v>28</v>
       </c>
       <c r="C178" t="s">
-        <v>459</v>
+        <v>367</v>
+      </c>
+      <c r="D178" t="s">
+        <v>384</v>
       </c>
       <c r="E178" t="s">
-        <v>134</v>
+        <v>439</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>308</v>
+        <v>463</v>
       </c>
       <c r="B179" t="s">
         <v>28</v>
       </c>
       <c r="C179" t="s">
-        <v>325</v>
+        <v>368</v>
       </c>
       <c r="D179" t="s">
-        <v>309</v>
+        <v>364</v>
       </c>
       <c r="E179" t="s">
-        <v>344</v>
+        <v>159</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>308</v>
+        <v>463</v>
       </c>
       <c r="B180" t="s">
         <v>28</v>
       </c>
       <c r="C180" t="s">
-        <v>326</v>
+        <v>369</v>
       </c>
       <c r="D180" t="s">
-        <v>329</v>
+        <v>385</v>
       </c>
       <c r="E180" t="s">
-        <v>345</v>
+        <v>160</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>308</v>
+        <v>463</v>
       </c>
       <c r="B181" t="s">
         <v>28</v>
       </c>
       <c r="C181" t="s">
-        <v>327</v>
+        <v>235</v>
       </c>
       <c r="D181" t="s">
-        <v>334</v>
+        <v>365</v>
       </c>
       <c r="E181" t="s">
-        <v>346</v>
+        <v>161</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>308</v>
+        <v>463</v>
       </c>
       <c r="B182" t="s">
         <v>28</v>
       </c>
       <c r="C182" t="s">
-        <v>328</v>
+        <v>236</v>
       </c>
       <c r="D182" t="s">
-        <v>330</v>
+        <v>386</v>
       </c>
       <c r="E182" t="s">
-        <v>85</v>
+        <v>162</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>308</v>
+        <v>463</v>
       </c>
       <c r="B183" t="s">
         <v>28</v>
       </c>
       <c r="C183" t="s">
-        <v>339</v>
-      </c>
-      <c r="D183" t="s">
-        <v>335</v>
+        <v>458</v>
       </c>
       <c r="E183" t="s">
-        <v>86</v>
+        <v>133</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>308</v>
+        <v>463</v>
       </c>
       <c r="B184" t="s">
         <v>28</v>
       </c>
       <c r="C184" t="s">
-        <v>340</v>
-      </c>
-      <c r="D184" t="s">
-        <v>331</v>
+        <v>459</v>
       </c>
       <c r="E184" t="s">
-        <v>44</v>
+        <v>134</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -4951,13 +4979,13 @@
         <v>28</v>
       </c>
       <c r="C185" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="D185" t="s">
-        <v>336</v>
+        <v>309</v>
       </c>
       <c r="E185" t="s">
-        <v>45</v>
+        <v>344</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -4968,13 +4996,13 @@
         <v>28</v>
       </c>
       <c r="C186" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="D186" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E186" t="s">
-        <v>87</v>
+        <v>345</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -4985,13 +5013,13 @@
         <v>28</v>
       </c>
       <c r="C187" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="D187" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E187" t="s">
-        <v>88</v>
+        <v>346</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -5002,13 +5030,13 @@
         <v>28</v>
       </c>
       <c r="C188" t="s">
-        <v>16</v>
+        <v>328</v>
       </c>
       <c r="D188" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="E188" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -5019,13 +5047,13 @@
         <v>28</v>
       </c>
       <c r="C189" t="s">
-        <v>17</v>
+        <v>339</v>
       </c>
       <c r="D189" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E189" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -5036,13 +5064,13 @@
         <v>28</v>
       </c>
       <c r="C190" t="s">
-        <v>18</v>
+        <v>340</v>
       </c>
       <c r="D190" t="s">
-        <v>192</v>
+        <v>331</v>
       </c>
       <c r="E190" t="s">
-        <v>347</v>
+        <v>44</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -5053,13 +5081,13 @@
         <v>28</v>
       </c>
       <c r="C191" t="s">
-        <v>19</v>
+        <v>341</v>
       </c>
       <c r="D191" t="s">
-        <v>209</v>
+        <v>336</v>
       </c>
       <c r="E191" t="s">
-        <v>348</v>
+        <v>45</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5070,13 +5098,13 @@
         <v>28</v>
       </c>
       <c r="C192" t="s">
-        <v>20</v>
+        <v>342</v>
       </c>
       <c r="D192" t="s">
-        <v>193</v>
+        <v>332</v>
       </c>
       <c r="E192" t="s">
-        <v>129</v>
+        <v>87</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -5087,183 +5115,171 @@
         <v>28</v>
       </c>
       <c r="C193" t="s">
-        <v>21</v>
+        <v>343</v>
       </c>
       <c r="D193" t="s">
-        <v>210</v>
+        <v>337</v>
       </c>
       <c r="E193" t="s">
-        <v>130</v>
+        <v>88</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>168</v>
+        <v>308</v>
       </c>
       <c r="B194" t="s">
         <v>28</v>
       </c>
       <c r="C194" t="s">
-        <v>227</v>
+        <v>16</v>
       </c>
       <c r="D194" t="s">
-        <v>169</v>
+        <v>333</v>
       </c>
       <c r="E194" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>168</v>
+        <v>308</v>
       </c>
       <c r="B195" t="s">
         <v>28</v>
       </c>
       <c r="C195" t="s">
-        <v>228</v>
+        <v>17</v>
       </c>
       <c r="D195" t="s">
-        <v>170</v>
+        <v>338</v>
       </c>
       <c r="E195" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>168</v>
+        <v>308</v>
       </c>
       <c r="B196" t="s">
         <v>28</v>
       </c>
       <c r="C196" t="s">
-        <v>229</v>
+        <v>18</v>
       </c>
       <c r="D196" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="E196" t="s">
-        <v>251</v>
+        <v>347</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>168</v>
+        <v>308</v>
       </c>
       <c r="B197" t="s">
         <v>28</v>
       </c>
       <c r="C197" t="s">
-        <v>230</v>
+        <v>19</v>
       </c>
       <c r="D197" t="s">
-        <v>172</v>
+        <v>209</v>
       </c>
       <c r="E197" t="s">
-        <v>42</v>
+        <v>348</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>168</v>
+        <v>308</v>
       </c>
       <c r="B198" t="s">
         <v>28</v>
       </c>
       <c r="C198" t="s">
-        <v>231</v>
+        <v>20</v>
       </c>
       <c r="D198" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="E198" t="s">
-        <v>46</v>
+        <v>129</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>168</v>
+        <v>308</v>
       </c>
       <c r="B199" t="s">
         <v>28</v>
       </c>
       <c r="C199" t="s">
-        <v>232</v>
+        <v>21</v>
       </c>
       <c r="D199" t="s">
-        <v>174</v>
+        <v>210</v>
       </c>
       <c r="E199" t="s">
-        <v>252</v>
+        <v>130</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>168</v>
+        <v>308</v>
       </c>
       <c r="B200" t="s">
         <v>28</v>
       </c>
       <c r="C200" t="s">
-        <v>233</v>
-      </c>
-      <c r="D200" t="s">
-        <v>175</v>
+        <v>12</v>
       </c>
       <c r="E200" t="s">
-        <v>253</v>
+        <v>464</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>168</v>
+        <v>308</v>
       </c>
       <c r="B201" t="s">
         <v>28</v>
       </c>
       <c r="C201" t="s">
-        <v>234</v>
-      </c>
-      <c r="D201" t="s">
-        <v>176</v>
+        <v>13</v>
       </c>
       <c r="E201" t="s">
-        <v>254</v>
+        <v>465</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>168</v>
+        <v>308</v>
       </c>
       <c r="B202" t="s">
         <v>28</v>
       </c>
       <c r="C202" t="s">
-        <v>18</v>
-      </c>
-      <c r="D202" t="s">
-        <v>192</v>
+        <v>458</v>
       </c>
       <c r="E202" t="s">
-        <v>58</v>
+        <v>466</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>168</v>
+        <v>308</v>
       </c>
       <c r="B203" t="s">
         <v>28</v>
       </c>
       <c r="C203" t="s">
-        <v>19</v>
-      </c>
-      <c r="D203" t="s">
-        <v>209</v>
+        <v>459</v>
       </c>
       <c r="E203" t="s">
-        <v>59</v>
+        <v>467</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -5274,13 +5290,13 @@
         <v>28</v>
       </c>
       <c r="C204" t="s">
-        <v>20</v>
+        <v>227</v>
       </c>
       <c r="D204" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="E204" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -5291,13 +5307,13 @@
         <v>28</v>
       </c>
       <c r="C205" t="s">
-        <v>21</v>
+        <v>228</v>
       </c>
       <c r="D205" t="s">
-        <v>210</v>
+        <v>170</v>
       </c>
       <c r="E205" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
@@ -5308,13 +5324,13 @@
         <v>28</v>
       </c>
       <c r="C206" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="D206" t="s">
-        <v>211</v>
+        <v>171</v>
       </c>
       <c r="E206" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -5325,13 +5341,13 @@
         <v>28</v>
       </c>
       <c r="C207" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D207" t="s">
-        <v>212</v>
+        <v>172</v>
       </c>
       <c r="E207" t="s">
-        <v>256</v>
+        <v>42</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -5342,13 +5358,13 @@
         <v>28</v>
       </c>
       <c r="C208" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D208" t="s">
-        <v>213</v>
+        <v>173</v>
       </c>
       <c r="E208" t="s">
-        <v>257</v>
+        <v>46</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -5359,13 +5375,13 @@
         <v>28</v>
       </c>
       <c r="C209" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D209" t="s">
-        <v>214</v>
+        <v>174</v>
       </c>
       <c r="E209" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -5376,13 +5392,13 @@
         <v>28</v>
       </c>
       <c r="C210" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="D210" t="s">
-        <v>215</v>
+        <v>175</v>
       </c>
       <c r="E210" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -5393,13 +5409,13 @@
         <v>28</v>
       </c>
       <c r="C211" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D211" t="s">
-        <v>216</v>
+        <v>176</v>
       </c>
       <c r="E211" t="s">
-        <v>137</v>
+        <v>254</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -5410,13 +5426,13 @@
         <v>28</v>
       </c>
       <c r="C212" t="s">
-        <v>241</v>
+        <v>18</v>
       </c>
       <c r="D212" t="s">
-        <v>217</v>
+        <v>192</v>
       </c>
       <c r="E212" t="s">
-        <v>260</v>
+        <v>58</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -5427,13 +5443,13 @@
         <v>28</v>
       </c>
       <c r="C213" t="s">
-        <v>242</v>
+        <v>19</v>
       </c>
       <c r="D213" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E213" t="s">
-        <v>139</v>
+        <v>59</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -5444,13 +5460,13 @@
         <v>28</v>
       </c>
       <c r="C214" t="s">
-        <v>243</v>
+        <v>20</v>
       </c>
       <c r="D214" t="s">
-        <v>219</v>
+        <v>193</v>
       </c>
       <c r="E214" t="s">
-        <v>261</v>
+        <v>60</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -5461,13 +5477,13 @@
         <v>28</v>
       </c>
       <c r="C215" t="s">
-        <v>244</v>
+        <v>21</v>
       </c>
       <c r="D215" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="E215" t="s">
-        <v>262</v>
+        <v>61</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -5478,13 +5494,13 @@
         <v>28</v>
       </c>
       <c r="C216" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="D216" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="E216" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -5495,13 +5511,13 @@
         <v>28</v>
       </c>
       <c r="C217" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="D217" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="E217" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
@@ -5512,13 +5528,13 @@
         <v>28</v>
       </c>
       <c r="C218" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="D218" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="E218" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -5529,13 +5545,13 @@
         <v>28</v>
       </c>
       <c r="C219" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="D219" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="E219" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -5546,13 +5562,13 @@
         <v>28</v>
       </c>
       <c r="C220" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="D220" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="E220" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
@@ -5563,75 +5579,189 @@
         <v>28</v>
       </c>
       <c r="C221" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="D221" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="E221" t="s">
-        <v>268</v>
+        <v>137</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>308</v>
+        <v>168</v>
       </c>
       <c r="B222" t="s">
         <v>28</v>
       </c>
       <c r="C222" t="s">
-        <v>12</v>
+        <v>241</v>
+      </c>
+      <c r="D222" t="s">
+        <v>217</v>
       </c>
       <c r="E222" t="s">
-        <v>464</v>
+        <v>260</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>308</v>
+        <v>168</v>
       </c>
       <c r="B223" t="s">
         <v>28</v>
       </c>
       <c r="C223" t="s">
-        <v>13</v>
+        <v>242</v>
+      </c>
+      <c r="D223" t="s">
+        <v>218</v>
       </c>
       <c r="E223" t="s">
-        <v>465</v>
+        <v>139</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>308</v>
+        <v>168</v>
       </c>
       <c r="B224" t="s">
         <v>28</v>
       </c>
       <c r="C224" t="s">
-        <v>458</v>
+        <v>243</v>
+      </c>
+      <c r="D224" t="s">
+        <v>219</v>
       </c>
       <c r="E224" t="s">
-        <v>466</v>
+        <v>261</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>308</v>
+        <v>168</v>
       </c>
       <c r="B225" t="s">
         <v>28</v>
       </c>
       <c r="C225" t="s">
-        <v>459</v>
+        <v>244</v>
+      </c>
+      <c r="D225" t="s">
+        <v>222</v>
       </c>
       <c r="E225" t="s">
-        <v>467</v>
+        <v>262</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>168</v>
+      </c>
+      <c r="B226" t="s">
+        <v>28</v>
+      </c>
+      <c r="C226" t="s">
+        <v>245</v>
+      </c>
+      <c r="D226" t="s">
+        <v>221</v>
+      </c>
+      <c r="E226" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>168</v>
+      </c>
+      <c r="B227" t="s">
+        <v>28</v>
+      </c>
+      <c r="C227" t="s">
+        <v>246</v>
+      </c>
+      <c r="D227" t="s">
+        <v>220</v>
+      </c>
+      <c r="E227" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>168</v>
+      </c>
+      <c r="B228" t="s">
+        <v>28</v>
+      </c>
+      <c r="C228" t="s">
+        <v>247</v>
+      </c>
+      <c r="D228" t="s">
+        <v>223</v>
+      </c>
+      <c r="E228" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>168</v>
+      </c>
+      <c r="B229" t="s">
+        <v>28</v>
+      </c>
+      <c r="C229" t="s">
+        <v>248</v>
+      </c>
+      <c r="D229" t="s">
+        <v>224</v>
+      </c>
+      <c r="E229" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>168</v>
+      </c>
+      <c r="B230" t="s">
+        <v>28</v>
+      </c>
+      <c r="C230" t="s">
+        <v>249</v>
+      </c>
+      <c r="D230" t="s">
+        <v>225</v>
+      </c>
+      <c r="E230" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>168</v>
+      </c>
+      <c r="B231" t="s">
+        <v>28</v>
+      </c>
+      <c r="C231" t="s">
+        <v>250</v>
+      </c>
+      <c r="D231" t="s">
+        <v>226</v>
+      </c>
+      <c r="E231" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E225" xr:uid="{5AC65239-A95B-4A8F-9499-495761FDA170}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E221">
-      <sortCondition ref="A1:A221"/>
+  <autoFilter ref="A1:E231" xr:uid="{5AC65239-A95B-4A8F-9499-495761FDA170}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E231">
+      <sortCondition ref="A1:A231"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>